<commit_message>
Add additional console results
</commit_message>
<xml_diff>
--- a/Assignment 01/Results.xlsx
+++ b/Assignment 01/Results.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9bfbbf63dbcedf51/Documents/J97 - Master of Cyber Security/CYB6009-Data-Analysis-and-Visualisation/Assignment 01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="8_{00B3C0D6-BF64-455F-A1B0-892C88C64FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82C1CE4B-7EFA-4377-AFBA-356949B305D3}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="8_{00B3C0D6-BF64-455F-A1B0-892C88C64FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BB3730-6F5B-4EE3-B5B1-DE006B96D7D4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{BECBC701-2CF7-4E3B-AE25-81D3BF68531B}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{BECBC701-2CF7-4E3B-AE25-81D3BF68531B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Categorical &amp; Binary Features" sheetId="1" r:id="rId1"/>
+    <sheet name="Continuous Features" sheetId="2" r:id="rId2"/>
+    <sheet name="Coefficients (Loadings)" sheetId="3" r:id="rId3"/>
+    <sheet name="Cumulative Proportions" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Categorical &amp; Binary Features'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Continuous Features'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>Categorical Feature</t>
   </si>
@@ -170,6 +172,33 @@
   </si>
   <si>
     <t>0(0.00%)</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC2</t>
+  </si>
+  <si>
+    <t>PC3</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Proportion of Variance</t>
+  </si>
+  <si>
+    <t>Cumulative Proportion</t>
+  </si>
+  <si>
+    <t>Loadings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Importance of components:</t>
   </si>
 </sst>
 </file>
@@ -233,7 +262,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -251,35 +280,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -290,39 +290,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -346,38 +313,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -697,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AE143C-74C9-4D3D-B5F8-B7E77A792EB8}">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="A1:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,414 +685,298 @@
     <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="3">
         <v>264</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="22">
         <v>0.44</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="11" t="s">
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="17">
         <v>238</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="18">
         <v>0.39700000000000002</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="3"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="11" t="s">
+      <c r="H3" s="8"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="17">
         <v>54</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="18">
         <v>0.09</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="3"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="11" t="s">
+      <c r="H4" s="8"/>
+      <c r="O4" s="1"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="17">
         <v>40</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="18">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="3"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="14" t="s">
+      <c r="H5" s="8"/>
+      <c r="O5" s="1"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="24">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="3"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="H6" s="8"/>
+      <c r="O6" s="1"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="3">
         <v>397</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="22">
         <v>0.66200000000000003</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="3"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="11" t="s">
+      <c r="O7" s="1"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="17">
         <v>177</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="18">
         <v>0.29499999999999998</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="3"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="11" t="s">
+      <c r="O8" s="1"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="17">
         <v>13</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="18">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="3"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="14" t="s">
+      <c r="O9" s="1"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="2">
         <v>13</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="24">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="3"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="O10" s="1"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="3">
         <v>396</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="22">
         <v>0.66</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="3"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="11" t="s">
+      <c r="H11" s="8"/>
+      <c r="O11" s="1"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="17">
         <v>151</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="18">
         <v>0.252</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="3"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="14" t="s">
+      <c r="H12" s="8"/>
+      <c r="O12" s="1"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="2">
         <v>53</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="24">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="3">
         <v>365</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="22">
         <v>0.60799999999999998</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="14" t="s">
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="2">
         <v>235</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="24">
         <v>0.39200000000000002</v>
       </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="3">
         <v>300</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="22">
         <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="2">
         <v>300</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="24">
         <v>0.5</v>
       </c>
     </row>
@@ -1147,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AFBB51-2EE8-4BC4-B63E-21EAE222A8AE}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,235 +1010,233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="27" t="s">
-        <v>40</v>
-      </c>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="12">
         <v>-1</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="12">
         <v>80580</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="12">
         <v>48476.33</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="12">
         <v>49268.5</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="12">
         <v>-0.28000000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="12">
         <v>0.19</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="12">
         <v>0.92</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="12">
         <v>0.61</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="12">
         <v>0.63</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="12">
         <v>-0.56999999999999995</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="12">
         <v>76495</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="12">
         <v>822051</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="12">
         <v>492667.72</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="12">
         <v>492937</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="12">
         <v>-0.06</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="12">
         <v>119</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="12">
         <v>415</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="12">
         <v>267.75</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="12">
         <v>267</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="12">
         <v>-0.04</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="12">
         <v>0.02</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="12">
         <v>1821.42</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="12">
         <v>432.24</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="12">
         <v>399.72</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="12">
         <v>0.95</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="12">
         <v>75</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="12">
         <v>417</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="12">
         <v>226.75</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="12">
         <v>221</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="12">
         <v>0.23</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="12">
         <v>1260</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="12">
         <v>1439</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="12">
         <v>1349.68</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="12">
         <v>1348</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="12">
         <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="12">
         <v>32</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="12">
         <v>108</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="12">
         <v>63.98</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="12">
         <v>63</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="12">
         <v>0.19</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="15">
         <v>9</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="15">
         <v>34</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="15">
         <v>21.37</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="15">
         <v>21.5</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="15">
         <v>-0.03</v>
       </c>
     </row>
@@ -1399,4 +1244,248 @@
   <autoFilter ref="A1:G1" xr:uid="{E9AFBB51-2EE8-4BC4-B63E-21EAE222A8AE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4319F87A-5877-4CD6-BA02-307F179DF6A4}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="17">
+        <v>-0.56126977</v>
+      </c>
+      <c r="C2" s="17">
+        <v>0.19729622999999999</v>
+      </c>
+      <c r="D2" s="17">
+        <v>2.8131679999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="17">
+        <v>0.52351435000000002</v>
+      </c>
+      <c r="C3" s="17">
+        <v>0.26940545999999999</v>
+      </c>
+      <c r="D3" s="17">
+        <v>2.8585630000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="17">
+        <v>-2.5642080000000001E-2</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1.8161420000000001E-2</v>
+      </c>
+      <c r="D4" s="17">
+        <v>0.74665649999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="17">
+        <v>-1.932975E-2</v>
+      </c>
+      <c r="C5" s="17">
+        <v>6.1024189999999999E-2</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.45832918</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="17">
+        <v>-0.19866866999999999</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0.53762356</v>
+      </c>
+      <c r="D6" s="17">
+        <v>-0.17961167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="17">
+        <v>0.58639671000000004</v>
+      </c>
+      <c r="C7" s="17">
+        <v>-7.0569380000000001E-2</v>
+      </c>
+      <c r="D7" s="17">
+        <v>-1.167788E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="17">
+        <v>6.5768279999999998E-2</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0.12188453</v>
+      </c>
+      <c r="D8" s="17">
+        <v>-0.34287830000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="17">
+        <v>5.4396460000000001E-2</v>
+      </c>
+      <c r="C9" s="17">
+        <v>0.15549594999999999</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0.27940290000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.13879131</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.74255446999999997</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5.2930789999999998E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44F915C-50CF-496F-8B56-D0AE1C30CE65}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="17">
+        <v>1.5256000000000001</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1.1617</v>
+      </c>
+      <c r="D2" s="17">
+        <v>1.0170999999999999</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0.98240000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="17">
+        <v>0.2586</v>
+      </c>
+      <c r="C3" s="17">
+        <v>0.14990000000000001</v>
+      </c>
+      <c r="D3" s="17">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0.1149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.2586</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.40849999999999997</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.52890000000000004</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.64390000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>